<commit_message>
Implemented Excel writeline functionality
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,9 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Fri Jun 10 18:28:09 2022</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Dr. John Doe</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>2022-06-04</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -327,19 +339,35 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3"/>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>